<commit_message>
Fix typo, add function to check current shortcuts
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DRIVE - dat.huynhthong\My Drive\Codes\shortcut-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA93CE0E-F1A9-4F6C-BC97-9113043D0C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78DE561-6094-421F-955B-226D62D37EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{824FD941-DF03-42E5-B5D7-633A14B5EB52}"/>
   </bookViews>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add function to create shortcuts from stored data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DRIVE - dat.huynhthong\My Drive\Codes\shortcut-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E654A7-83F7-416A-B729-397DED57B914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E1E9FA-82DA-4BF7-93F7-F61661C6FF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{824FD941-DF03-42E5-B5D7-633A14B5EB52}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>groupName</t>
   </si>
@@ -43,110 +56,155 @@
     <t>Google</t>
   </si>
   <si>
-    <t>google.com</t>
-  </si>
-  <si>
     <t>YouTube</t>
   </si>
   <si>
-    <t>youtube.com</t>
-  </si>
-  <si>
     <t>Facebook</t>
   </si>
   <si>
-    <t>facebook.com</t>
-  </si>
-  <si>
     <t>Instagram</t>
   </si>
   <si>
-    <t>instagram.com</t>
-  </si>
-  <si>
     <t>WhatsApp</t>
   </si>
   <si>
-    <t>whatsapp.com</t>
-  </si>
-  <si>
     <t>X (formerly Twitter)</t>
   </si>
   <si>
-    <t>x.com</t>
-  </si>
-  <si>
     <t>Wikipedia</t>
   </si>
   <si>
-    <t>wikipedia.org</t>
-  </si>
-  <si>
     <t>ChatGPT</t>
   </si>
   <si>
-    <t>chatgpt.com</t>
-  </si>
-  <si>
     <t>Reddit</t>
   </si>
   <si>
-    <t>reddit.com</t>
-  </si>
-  <si>
     <t>Yahoo</t>
   </si>
   <si>
-    <t>yahoo.com</t>
-  </si>
-  <si>
     <t>SUPP</t>
   </si>
   <si>
     <t>Amazon</t>
   </si>
   <si>
-    <t>amazon.com</t>
-  </si>
-  <si>
     <t>LinkedIn</t>
   </si>
   <si>
-    <t>linkedin.com</t>
-  </si>
-  <si>
     <t>Netflix</t>
   </si>
   <si>
-    <t>netflix.com</t>
-  </si>
-  <si>
     <t>eBay</t>
   </si>
   <si>
-    <t>ebay.com</t>
-  </si>
-  <si>
     <t>Pinterest</t>
   </si>
   <si>
-    <t>pinterest.com</t>
-  </si>
-  <si>
-    <t>dsd</t>
-  </si>
-  <si>
     <t>#6c8d91</t>
   </si>
   <si>
-    <t>#2d9268</t>
+    <t>groupID</t>
+  </si>
+  <si>
+    <t>group-1</t>
+  </si>
+  <si>
+    <t>group-2</t>
+  </si>
+  <si>
+    <t>https://www.google.com/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/</t>
+  </si>
+  <si>
+    <t>https://www.whatsapp.com/</t>
+  </si>
+  <si>
+    <t>https://www.x.com/</t>
+  </si>
+  <si>
+    <t>https://www.wikipedia.org/</t>
+  </si>
+  <si>
+    <t>https://www.chatgpt.com/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/</t>
+  </si>
+  <si>
+    <t>https://www.yahoo.com/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/</t>
+  </si>
+  <si>
+    <t>https://www.netflix.com/</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/</t>
+  </si>
+  <si>
+    <t>https://www.pinterest.com/</t>
+  </si>
+  <si>
+    <t>#F39C12</t>
+  </si>
+  <si>
+    <t>#E74C3C</t>
+  </si>
+  <si>
+    <t>#8E44AD</t>
+  </si>
+  <si>
+    <t>#3498DB</t>
+  </si>
+  <si>
+    <t>#2ECC71</t>
+  </si>
+  <si>
+    <t>#D35400</t>
+  </si>
+  <si>
+    <t>#C0392B</t>
+  </si>
+  <si>
+    <t>#27AE60</t>
+  </si>
+  <si>
+    <t>#2980B9</t>
+  </si>
+  <si>
+    <t>#F1C40F</t>
+  </si>
+  <si>
+    <t>#E67E22</t>
+  </si>
+  <si>
+    <t>#1ABC9C</t>
+  </si>
+  <si>
+    <t>#34495E</t>
+  </si>
+  <si>
+    <t>#7D3C98</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +335,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1000,211 +1064,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEF550E-0339-4A47-BC65-70C07CCC91A5}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
       <c r="E9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
+      <c r="B12" t="s">
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add functions checkAndAddBlankShortcuts and rearrangeGroupIds
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DRIVE - dat.huynhthong\My Drive\Codes\shortcut-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E1E9FA-82DA-4BF7-93F7-F61661C6FF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BF7F33-622E-449B-BA24-29D97B2223B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{824FD941-DF03-42E5-B5D7-633A14B5EB52}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
   <si>
     <t>groupName</t>
   </si>
@@ -197,7 +197,7 @@
     <t>#34495E</t>
   </si>
   <si>
-    <t>#7D3C98</t>
+    <t>#e8a5a0</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,6 +1302,9 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
       <c r="D12" t="s">
         <v>17</v>
       </c>
@@ -1319,6 +1322,9 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
       <c r="D13" t="s">
         <v>18</v>
       </c>
@@ -1336,6 +1342,9 @@
       <c r="B14" t="s">
         <v>16</v>
       </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -1353,6 +1362,9 @@
       <c r="B15" t="s">
         <v>16</v>
       </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
@@ -1370,7 +1382,7 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="F16" t="s">
+      <c r="C16" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1380,6 +1392,9 @@
       </c>
       <c r="B17" t="s">
         <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Add function to add blank group
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DRIVE - dat.huynhthong\My Drive\Codes\shortcut-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BF7F33-622E-449B-BA24-29D97B2223B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9420B4FA-1D82-4233-A81A-FC420CD7FDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{824FD941-DF03-42E5-B5D7-633A14B5EB52}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>groupName</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>#e8a5a0</t>
+  </si>
+  <si>
+    <t>group-3</t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEF550E-0339-4A47-BC65-70C07CCC91A5}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,25 +1302,10 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -1326,18 +1314,18 @@
         <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -1346,18 +1334,18 @@
         <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1366,18 +1354,18 @@
         <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -1385,10 +1373,19 @@
       <c r="C16" t="s">
         <v>54</v>
       </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1396,13 +1393,24 @@
       <c r="C17" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add delete function, style target element
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DRIVE - dat.huynhthong\My Drive\Codes\shortcut-extension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DRIVE - dat.huynhthong\My Drive\Codes\d-route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9420B4FA-1D82-4233-A81A-FC420CD7FDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B670F2B6-F973-4B37-AF9B-6DA088877A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{824FD941-DF03-42E5-B5D7-633A14B5EB52}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
   <si>
     <t>groupName</t>
   </si>
@@ -201,6 +201,15 @@
   </si>
   <si>
     <t>group-3</t>
+  </si>
+  <si>
+    <t>group-4</t>
+  </si>
+  <si>
+    <t>MAIN 2</t>
+  </si>
+  <si>
+    <t>SUPP 2</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEF550E-0339-4A47-BC65-70C07CCC91A5}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,10 +1209,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -1220,10 +1229,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1240,10 +1249,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -1260,10 +1269,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -1280,10 +1289,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -1300,117 +1309,121 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
         <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
         <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
         <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F17" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>